<commit_message>
ICR rejection m errorbars
</commit_message>
<xml_diff>
--- a/data/ICR/IC_data_ICR_udvalgtdata_igen.xlsx
+++ b/data/ICR/IC_data_ICR_udvalgtdata_igen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102222\OneDrive - Grundfos\Desktop\Speciale\data\ICR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/ICR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04B00EE-9CB3-4486-9718-9FF85EACF38C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B04B00EE-9CB3-4486-9718-9FF85EACF38C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{95D76E44-5EB7-44F7-AD9F-623AF2676821}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1251AAB3-9298-4E56-BCEC-410086F0A626}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{1251AAB3-9298-4E56-BCEC-410086F0A626}"/>
   </bookViews>
   <sheets>
     <sheet name="data Cl" sheetId="7" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="data Na" sheetId="1" r:id="rId3"/>
     <sheet name="data Ca" sheetId="11" r:id="rId4"/>
     <sheet name="data Mg" sheetId="4" r:id="rId5"/>
-    <sheet name="std Cl" sheetId="8" r:id="rId6"/>
-    <sheet name="std SO4" sheetId="10" r:id="rId7"/>
-    <sheet name="std Na" sheetId="2" r:id="rId8"/>
-    <sheet name="std Ca " sheetId="12" r:id="rId9"/>
-    <sheet name="std mg" sheetId="5" r:id="rId10"/>
+    <sheet name="data SiO2" sheetId="13" r:id="rId6"/>
+    <sheet name="std Cl" sheetId="8" r:id="rId7"/>
+    <sheet name="std SO4" sheetId="10" r:id="rId8"/>
+    <sheet name="std Na" sheetId="2" r:id="rId9"/>
+    <sheet name="std Ca " sheetId="12" r:id="rId10"/>
+    <sheet name="std mg" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="44">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -153,13 +154,7 @@
     <t>dilution</t>
   </si>
   <si>
-    <t>feed</t>
-  </si>
-  <si>
     <t xml:space="preserve">stream </t>
-  </si>
-  <si>
-    <t>Permeat</t>
   </si>
   <si>
     <t>Perm spand</t>
@@ -173,12 +168,21 @@
   <si>
     <t>2 [mg/L]</t>
   </si>
+  <si>
+    <t>SiO2 [mg/l]</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>Permeate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +190,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,10 +237,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6692,8 +6719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7652B623-3E84-4605-8EBF-152B8F916C54}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6703,19 +6730,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6723,7 +6750,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6740,7 +6767,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -6757,7 +6784,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -6774,7 +6801,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -6791,7 +6818,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -6808,7 +6835,7 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -6825,7 +6852,7 @@
         <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -6842,7 +6869,7 @@
         <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -6859,7 +6886,7 @@
         <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -6876,7 +6903,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -6893,7 +6920,7 @@
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -6910,7 +6937,7 @@
         <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -6927,7 +6954,7 @@
         <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -6944,7 +6971,7 @@
         <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -6961,7 +6988,7 @@
         <v>300</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -6978,7 +7005,7 @@
         <v>360</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2">
         <v>5</v>
@@ -6992,10 +7019,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>400</v>
+        <f>8*60</f>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
@@ -7012,7 +7040,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -7029,7 +7057,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -7046,7 +7074,7 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -7063,7 +7091,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -7080,7 +7108,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -7097,7 +7125,7 @@
         <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -7114,7 +7142,7 @@
         <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -7131,7 +7159,7 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -7148,7 +7176,7 @@
         <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -7165,7 +7193,7 @@
         <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -7182,7 +7210,7 @@
         <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -7199,7 +7227,7 @@
         <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -7216,7 +7244,7 @@
         <v>270</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -7233,7 +7261,7 @@
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -7250,7 +7278,7 @@
         <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -7267,7 +7295,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -7284,7 +7312,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -7301,7 +7329,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -7320,6 +7348,845 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436A1398-863C-424C-AD55-006B45D32DF9}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>9.1969999999999992</v>
+      </c>
+      <c r="E5">
+        <v>6.4088000000000003</v>
+      </c>
+      <c r="F5">
+        <v>25.02</v>
+      </c>
+      <c r="G5">
+        <v>15.42</v>
+      </c>
+      <c r="H5">
+        <v>12.18</v>
+      </c>
+      <c r="I5">
+        <v>24.935300000000002</v>
+      </c>
+      <c r="J5">
+        <f>(E5+0.0693)/0.26</f>
+        <v>24.915769230769232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>9.1969999999999992</v>
+      </c>
+      <c r="E6">
+        <v>6.4157999999999999</v>
+      </c>
+      <c r="F6">
+        <v>25.07</v>
+      </c>
+      <c r="G6">
+        <v>15.42</v>
+      </c>
+      <c r="H6">
+        <v>12.16</v>
+      </c>
+      <c r="I6">
+        <v>24.962199999999999</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J26" si="0">(E6+0.0693)/0.26</f>
+        <v>24.942692307692308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>9.2970000000000006</v>
+      </c>
+      <c r="E7">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>41.01</v>
+      </c>
+      <c r="G7">
+        <v>0.03</v>
+      </c>
+      <c r="H7">
+        <v>31.73</v>
+      </c>
+      <c r="I7">
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.32346153846153847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>9.3469999999999995</v>
+      </c>
+      <c r="E8">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F8">
+        <v>43.34</v>
+      </c>
+      <c r="G8">
+        <v>0.02</v>
+      </c>
+      <c r="H8">
+        <v>31.64</v>
+      </c>
+      <c r="I8">
+        <v>0.2298</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.29653846153846153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>9.31</v>
+      </c>
+      <c r="E9">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="F9">
+        <v>37.090000000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.01</v>
+      </c>
+      <c r="H9">
+        <v>23.16</v>
+      </c>
+      <c r="I9">
+        <v>0.2167</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.28346153846153843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>9.3469999999999995</v>
+      </c>
+      <c r="E10">
+        <v>3.3E-3</v>
+      </c>
+      <c r="F10">
+        <v>40.67</v>
+      </c>
+      <c r="G10">
+        <v>0.01</v>
+      </c>
+      <c r="H10">
+        <v>24.38</v>
+      </c>
+      <c r="I10">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0.27923076923076923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>9.33</v>
+      </c>
+      <c r="E11">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="F11">
+        <v>22.51</v>
+      </c>
+      <c r="G11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H11">
+        <v>11.13</v>
+      </c>
+      <c r="I11">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>1.0519230769230767</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>9.33</v>
+      </c>
+      <c r="E12">
+        <v>0.2198</v>
+      </c>
+      <c r="F12">
+        <v>23.13</v>
+      </c>
+      <c r="G12">
+        <v>0.59</v>
+      </c>
+      <c r="H12">
+        <v>11.62</v>
+      </c>
+      <c r="I12">
+        <v>1.0482</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1.111923076923077</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>2.5</v>
+      </c>
+      <c r="D13">
+        <v>9.32</v>
+      </c>
+      <c r="E13">
+        <v>0.59770000000000001</v>
+      </c>
+      <c r="F13">
+        <v>24.18</v>
+      </c>
+      <c r="G13">
+        <v>1.54</v>
+      </c>
+      <c r="H13">
+        <v>12.02</v>
+      </c>
+      <c r="I13">
+        <v>2.5066000000000002</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>2.5653846153846156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>2.5</v>
+      </c>
+      <c r="D14">
+        <v>9.32</v>
+      </c>
+      <c r="E14">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="F14">
+        <v>24.36</v>
+      </c>
+      <c r="G14">
+        <v>1.58</v>
+      </c>
+      <c r="H14">
+        <v>12.22</v>
+      </c>
+      <c r="I14">
+        <v>2.5451000000000001</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>2.6038461538461539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>9.31</v>
+      </c>
+      <c r="E15">
+        <v>1.2488999999999999</v>
+      </c>
+      <c r="F15">
+        <v>24.72</v>
+      </c>
+      <c r="G15">
+        <v>3.15</v>
+      </c>
+      <c r="H15">
+        <v>12.3</v>
+      </c>
+      <c r="I15">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>5.0699999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>9.31</v>
+      </c>
+      <c r="E16">
+        <v>1.2588999999999999</v>
+      </c>
+      <c r="F16">
+        <v>24.83</v>
+      </c>
+      <c r="G16">
+        <v>3.18</v>
+      </c>
+      <c r="H16">
+        <v>12.36</v>
+      </c>
+      <c r="I16">
+        <v>5.0585000000000004</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>5.1084615384615377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>9.2729999999999997</v>
+      </c>
+      <c r="E17">
+        <v>2.5065</v>
+      </c>
+      <c r="F17">
+        <v>24.85</v>
+      </c>
+      <c r="G17">
+        <v>6.22</v>
+      </c>
+      <c r="H17">
+        <v>12.24</v>
+      </c>
+      <c r="I17">
+        <v>9.8737999999999992</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>9.9069230769230767</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>9.2729999999999997</v>
+      </c>
+      <c r="E18">
+        <v>2.5215999999999998</v>
+      </c>
+      <c r="F18">
+        <v>24.94</v>
+      </c>
+      <c r="G18">
+        <v>6.25</v>
+      </c>
+      <c r="H18">
+        <v>12.28</v>
+      </c>
+      <c r="I18">
+        <v>9.9321000000000002</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>9.9649999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>9.1969999999999992</v>
+      </c>
+      <c r="E19">
+        <v>6.3742000000000001</v>
+      </c>
+      <c r="F19">
+        <v>24.98</v>
+      </c>
+      <c r="G19">
+        <v>15.36</v>
+      </c>
+      <c r="H19">
+        <v>12.15</v>
+      </c>
+      <c r="I19">
+        <v>24.8018</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>24.782692307692308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E20">
+        <v>6.4668999999999999</v>
+      </c>
+      <c r="F20">
+        <v>25.04</v>
+      </c>
+      <c r="G20">
+        <v>15.57</v>
+      </c>
+      <c r="H20">
+        <v>12.16</v>
+      </c>
+      <c r="I20">
+        <v>25.159700000000001</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>25.139230769230767</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>9.09</v>
+      </c>
+      <c r="E21">
+        <v>12.9101</v>
+      </c>
+      <c r="F21">
+        <v>25.24</v>
+      </c>
+      <c r="G21">
+        <v>29.47</v>
+      </c>
+      <c r="H21">
+        <v>12.01</v>
+      </c>
+      <c r="I21">
+        <v>50.027700000000003</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>49.920769230769231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>9.09</v>
+      </c>
+      <c r="E22">
+        <v>12.923400000000001</v>
+      </c>
+      <c r="F22">
+        <v>25.26</v>
+      </c>
+      <c r="G22">
+        <v>29.48</v>
+      </c>
+      <c r="H22">
+        <v>12.01</v>
+      </c>
+      <c r="I22">
+        <v>50.079000000000001</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>49.971923076923076</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>9.0069999999999997</v>
+      </c>
+      <c r="E23">
+        <v>19.258299999999998</v>
+      </c>
+      <c r="F23">
+        <v>25.28</v>
+      </c>
+      <c r="G23">
+        <v>41.68</v>
+      </c>
+      <c r="H23">
+        <v>11.79</v>
+      </c>
+      <c r="I23">
+        <v>74.529300000000006</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>74.336923076923057</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>75</v>
+      </c>
+      <c r="D24">
+        <v>9.0030000000000001</v>
+      </c>
+      <c r="E24">
+        <v>19.3248</v>
+      </c>
+      <c r="F24">
+        <v>25.31</v>
+      </c>
+      <c r="G24">
+        <v>41.75</v>
+      </c>
+      <c r="H24">
+        <v>11.83</v>
+      </c>
+      <c r="I24">
+        <v>74.786000000000001</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>74.592692307692303</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>8.9329999999999998</v>
+      </c>
+      <c r="E25">
+        <v>26.052600000000002</v>
+      </c>
+      <c r="F25">
+        <v>25.48</v>
+      </c>
+      <c r="G25">
+        <v>53.44</v>
+      </c>
+      <c r="H25">
+        <v>11.74</v>
+      </c>
+      <c r="I25">
+        <v>100.753</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>100.46884615384614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>8.9369999999999994</v>
+      </c>
+      <c r="E26">
+        <v>26.037199999999999</v>
+      </c>
+      <c r="F26">
+        <v>25.49</v>
+      </c>
+      <c r="G26">
+        <v>53.48</v>
+      </c>
+      <c r="H26">
+        <v>11.74</v>
+      </c>
+      <c r="I26">
+        <v>100.6932</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>100.40961538461536</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{F66653EC-FEAC-4B99-B4F1-A71418C72B42}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0.20419999999999999</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>26.1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E1:E26</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9275D82C-F64E-4922-BA73-8D1716E14925}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -8118,8 +8985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A934079E-BF22-4BA5-96F9-6264A094AA34}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8129,19 +8996,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8149,7 +9016,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -8166,7 +9033,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -8183,7 +9050,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -8200,7 +9067,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -8217,7 +9084,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -8234,7 +9101,7 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -8251,7 +9118,7 @@
         <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -8268,7 +9135,7 @@
         <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -8285,7 +9152,7 @@
         <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -8302,7 +9169,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -8319,7 +9186,7 @@
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -8336,7 +9203,7 @@
         <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -8353,7 +9220,7 @@
         <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -8370,7 +9237,7 @@
         <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -8387,7 +9254,7 @@
         <v>300</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -8404,7 +9271,7 @@
         <v>360</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2">
         <v>20</v>
@@ -8418,10 +9285,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>400</v>
+        <f>8*60</f>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>20</v>
@@ -8438,7 +9306,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -8455,7 +9323,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -8472,7 +9340,7 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -8489,7 +9357,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -8506,7 +9374,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -8523,7 +9391,7 @@
         <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -8540,7 +9408,7 @@
         <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -8557,7 +9425,7 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -8574,7 +9442,7 @@
         <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -8591,7 +9459,7 @@
         <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -8608,7 +9476,7 @@
         <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -8625,7 +9493,7 @@
         <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -8642,7 +9510,7 @@
         <v>270</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -8659,7 +9527,7 @@
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -8676,7 +9544,7 @@
         <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -8693,7 +9561,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -8710,7 +9578,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -8727,7 +9595,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -8743,9 +9611,6 @@
       <c r="A38">
         <v>60</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
       <c r="C38">
         <v>5</v>
       </c>
@@ -8760,9 +9625,6 @@
       <c r="A39">
         <v>120</v>
       </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
       <c r="C39">
         <v>5</v>
       </c>
@@ -8777,9 +9639,6 @@
       <c r="A40">
         <v>240</v>
       </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
       <c r="C40">
         <v>5</v>
       </c>
@@ -8794,9 +9653,6 @@
       <c r="A41">
         <v>60</v>
       </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
       <c r="C41">
         <v>1</v>
       </c>
@@ -8811,9 +9667,6 @@
       <c r="A42">
         <v>120</v>
       </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
       <c r="C42">
         <v>1</v>
       </c>
@@ -8827,9 +9680,6 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>240</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -8851,8 +9701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F79AAD-4066-48BF-8C0A-4FF64DF7561A}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8862,19 +9712,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8882,7 +9732,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -8899,7 +9749,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -8916,7 +9766,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -8933,7 +9783,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -8950,7 +9800,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -8967,7 +9817,7 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -8984,7 +9834,7 @@
         <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -9001,7 +9851,7 @@
         <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -9018,7 +9868,7 @@
         <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -9035,7 +9885,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -9052,7 +9902,7 @@
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -9069,7 +9919,7 @@
         <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -9086,7 +9936,7 @@
         <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -9103,7 +9953,7 @@
         <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -9120,7 +9970,7 @@
         <v>300</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -9137,7 +9987,7 @@
         <v>360</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1">
         <v>20</v>
@@ -9151,10 +10001,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>400</v>
+        <f>8*60</f>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1">
         <v>20</v>
@@ -9171,7 +10022,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -9188,7 +10039,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -9205,7 +10056,7 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -9222,7 +10073,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -9239,7 +10090,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -9256,7 +10107,7 @@
         <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -9273,7 +10124,7 @@
         <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -9290,7 +10141,7 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -9307,7 +10158,7 @@
         <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -9324,7 +10175,7 @@
         <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -9341,7 +10192,7 @@
         <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -9358,7 +10209,7 @@
         <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -9375,7 +10226,7 @@
         <v>270</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -9392,7 +10243,7 @@
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -9409,7 +10260,7 @@
         <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -9426,7 +10277,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -9443,7 +10294,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -9460,7 +10311,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -9482,8 +10333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C042B447-1565-4758-A623-46E782F17494}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9493,19 +10344,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9513,7 +10364,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -9530,7 +10381,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -9544,7 +10395,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -9561,7 +10412,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -9578,7 +10429,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -9595,7 +10446,7 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -9612,7 +10463,7 @@
         <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -9629,7 +10480,7 @@
         <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -9646,7 +10497,7 @@
         <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -9663,7 +10514,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -9680,7 +10531,7 @@
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -9697,7 +10548,7 @@
         <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -9714,7 +10565,7 @@
         <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -9731,7 +10582,7 @@
         <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -9748,7 +10599,7 @@
         <v>300</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -9765,7 +10616,7 @@
         <v>360</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2">
         <v>5</v>
@@ -9779,10 +10630,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>400</v>
+        <f>8*60</f>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
@@ -9799,7 +10651,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -9816,7 +10668,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -9833,7 +10685,7 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -9850,7 +10702,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -9867,7 +10719,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -9884,7 +10736,7 @@
         <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -9901,7 +10753,7 @@
         <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -9918,7 +10770,7 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -9935,7 +10787,7 @@
         <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -9952,7 +10804,7 @@
         <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -9969,7 +10821,7 @@
         <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -9986,7 +10838,7 @@
         <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -10000,7 +10852,7 @@
         <v>270</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -10017,7 +10869,7 @@
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -10034,7 +10886,7 @@
         <v>360</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -10051,7 +10903,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -10068,7 +10920,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -10085,7 +10937,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -10132,8 +10984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1ABD4B-85E3-4130-8AEB-4155DD23CD42}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10144,19 +10996,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10164,7 +11016,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -10181,7 +11033,7 @@
         <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -10198,7 +11050,7 @@
         <v>240</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -10215,7 +11067,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -10232,7 +11084,7 @@
         <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -10249,7 +11101,7 @@
         <v>240</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -10268,6 +11120,419 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDFB3A7-7363-48B1-AA7E-5E997504A952}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4">
+        <v>73.599999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4">
+        <v>73.599999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4">
+        <v>75.599999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4">
+        <v>77.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4">
+        <v>80.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>160</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>220</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4">
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>270</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4">
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>300</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>360</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>8*60</f>
+        <v>480</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4">
+        <v>104.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="4">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="4">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="4">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="4">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="4">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>140</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="4">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>220</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="4">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>240</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>270</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>300</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="4">
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>360</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="4">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="5">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4">
+        <v>54.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBFD0D1-E083-47A2-B457-A3132235FDA1}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -11087,7 +12352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74643F6B-09E9-4025-B309-D77977D1E381}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -11971,7 +13236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26414943-3047-4B83-AB1D-02EEB334AA0D}">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -12602,852 +13867,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436A1398-863C-424C-AD55-006B45D32DF9}">
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>9.1969999999999992</v>
-      </c>
-      <c r="E5">
-        <v>6.4088000000000003</v>
-      </c>
-      <c r="F5">
-        <v>25.02</v>
-      </c>
-      <c r="G5">
-        <v>15.42</v>
-      </c>
-      <c r="H5">
-        <v>12.18</v>
-      </c>
-      <c r="I5">
-        <v>24.935300000000002</v>
-      </c>
-      <c r="J5">
-        <f>(E5+0.0693)/0.26</f>
-        <v>24.915769230769232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>9.1969999999999992</v>
-      </c>
-      <c r="E6">
-        <v>6.4157999999999999</v>
-      </c>
-      <c r="F6">
-        <v>25.07</v>
-      </c>
-      <c r="G6">
-        <v>15.42</v>
-      </c>
-      <c r="H6">
-        <v>12.16</v>
-      </c>
-      <c r="I6">
-        <v>24.962199999999999</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ref="J6:J26" si="0">(E6+0.0693)/0.26</f>
-        <v>24.942692307692308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>9.2970000000000006</v>
-      </c>
-      <c r="E7">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="F7">
-        <v>41.01</v>
-      </c>
-      <c r="G7">
-        <v>0.03</v>
-      </c>
-      <c r="H7">
-        <v>31.73</v>
-      </c>
-      <c r="I7">
-        <v>0.25679999999999997</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>0.32346153846153847</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>9.3469999999999995</v>
-      </c>
-      <c r="E8">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="F8">
-        <v>43.34</v>
-      </c>
-      <c r="G8">
-        <v>0.02</v>
-      </c>
-      <c r="H8">
-        <v>31.64</v>
-      </c>
-      <c r="I8">
-        <v>0.2298</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0.29653846153846153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>9.31</v>
-      </c>
-      <c r="E9">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="F9">
-        <v>37.090000000000003</v>
-      </c>
-      <c r="G9">
-        <v>0.01</v>
-      </c>
-      <c r="H9">
-        <v>23.16</v>
-      </c>
-      <c r="I9">
-        <v>0.2167</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>0.28346153846153843</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>9.3469999999999995</v>
-      </c>
-      <c r="E10">
-        <v>3.3E-3</v>
-      </c>
-      <c r="F10">
-        <v>40.67</v>
-      </c>
-      <c r="G10">
-        <v>0.01</v>
-      </c>
-      <c r="H10">
-        <v>24.38</v>
-      </c>
-      <c r="I10">
-        <v>0.21249999999999999</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0.27923076923076923</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>9.33</v>
-      </c>
-      <c r="E11">
-        <v>0.20419999999999999</v>
-      </c>
-      <c r="F11">
-        <v>22.51</v>
-      </c>
-      <c r="G11">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H11">
-        <v>11.13</v>
-      </c>
-      <c r="I11">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>1.0519230769230767</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>9.33</v>
-      </c>
-      <c r="E12">
-        <v>0.2198</v>
-      </c>
-      <c r="F12">
-        <v>23.13</v>
-      </c>
-      <c r="G12">
-        <v>0.59</v>
-      </c>
-      <c r="H12">
-        <v>11.62</v>
-      </c>
-      <c r="I12">
-        <v>1.0482</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>1.111923076923077</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>2.5</v>
-      </c>
-      <c r="D13">
-        <v>9.32</v>
-      </c>
-      <c r="E13">
-        <v>0.59770000000000001</v>
-      </c>
-      <c r="F13">
-        <v>24.18</v>
-      </c>
-      <c r="G13">
-        <v>1.54</v>
-      </c>
-      <c r="H13">
-        <v>12.02</v>
-      </c>
-      <c r="I13">
-        <v>2.5066000000000002</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>2.5653846153846156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>2.5</v>
-      </c>
-      <c r="D14">
-        <v>9.32</v>
-      </c>
-      <c r="E14">
-        <v>0.60770000000000002</v>
-      </c>
-      <c r="F14">
-        <v>24.36</v>
-      </c>
-      <c r="G14">
-        <v>1.58</v>
-      </c>
-      <c r="H14">
-        <v>12.22</v>
-      </c>
-      <c r="I14">
-        <v>2.5451000000000001</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>2.6038461538461539</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>9.31</v>
-      </c>
-      <c r="E15">
-        <v>1.2488999999999999</v>
-      </c>
-      <c r="F15">
-        <v>24.72</v>
-      </c>
-      <c r="G15">
-        <v>3.15</v>
-      </c>
-      <c r="H15">
-        <v>12.3</v>
-      </c>
-      <c r="I15">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>5.0699999999999994</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>9.31</v>
-      </c>
-      <c r="E16">
-        <v>1.2588999999999999</v>
-      </c>
-      <c r="F16">
-        <v>24.83</v>
-      </c>
-      <c r="G16">
-        <v>3.18</v>
-      </c>
-      <c r="H16">
-        <v>12.36</v>
-      </c>
-      <c r="I16">
-        <v>5.0585000000000004</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>5.1084615384615377</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>9.2729999999999997</v>
-      </c>
-      <c r="E17">
-        <v>2.5065</v>
-      </c>
-      <c r="F17">
-        <v>24.85</v>
-      </c>
-      <c r="G17">
-        <v>6.22</v>
-      </c>
-      <c r="H17">
-        <v>12.24</v>
-      </c>
-      <c r="I17">
-        <v>9.8737999999999992</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>9.9069230769230767</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <v>9.2729999999999997</v>
-      </c>
-      <c r="E18">
-        <v>2.5215999999999998</v>
-      </c>
-      <c r="F18">
-        <v>24.94</v>
-      </c>
-      <c r="G18">
-        <v>6.25</v>
-      </c>
-      <c r="H18">
-        <v>12.28</v>
-      </c>
-      <c r="I18">
-        <v>9.9321000000000002</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>9.9649999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>9.1969999999999992</v>
-      </c>
-      <c r="E19">
-        <v>6.3742000000000001</v>
-      </c>
-      <c r="F19">
-        <v>24.98</v>
-      </c>
-      <c r="G19">
-        <v>15.36</v>
-      </c>
-      <c r="H19">
-        <v>12.15</v>
-      </c>
-      <c r="I19">
-        <v>24.8018</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>24.782692307692308</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="E20">
-        <v>6.4668999999999999</v>
-      </c>
-      <c r="F20">
-        <v>25.04</v>
-      </c>
-      <c r="G20">
-        <v>15.57</v>
-      </c>
-      <c r="H20">
-        <v>12.16</v>
-      </c>
-      <c r="I20">
-        <v>25.159700000000001</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>25.139230769230767</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
-      </c>
-      <c r="D21">
-        <v>9.09</v>
-      </c>
-      <c r="E21">
-        <v>12.9101</v>
-      </c>
-      <c r="F21">
-        <v>25.24</v>
-      </c>
-      <c r="G21">
-        <v>29.47</v>
-      </c>
-      <c r="H21">
-        <v>12.01</v>
-      </c>
-      <c r="I21">
-        <v>50.027700000000003</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>49.920769230769231</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>9.09</v>
-      </c>
-      <c r="E22">
-        <v>12.923400000000001</v>
-      </c>
-      <c r="F22">
-        <v>25.26</v>
-      </c>
-      <c r="G22">
-        <v>29.48</v>
-      </c>
-      <c r="H22">
-        <v>12.01</v>
-      </c>
-      <c r="I22">
-        <v>50.079000000000001</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>49.971923076923076</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23">
-        <v>75</v>
-      </c>
-      <c r="D23">
-        <v>9.0069999999999997</v>
-      </c>
-      <c r="E23">
-        <v>19.258299999999998</v>
-      </c>
-      <c r="F23">
-        <v>25.28</v>
-      </c>
-      <c r="G23">
-        <v>41.68</v>
-      </c>
-      <c r="H23">
-        <v>11.79</v>
-      </c>
-      <c r="I23">
-        <v>74.529300000000006</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>74.336923076923057</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24">
-        <v>75</v>
-      </c>
-      <c r="D24">
-        <v>9.0030000000000001</v>
-      </c>
-      <c r="E24">
-        <v>19.3248</v>
-      </c>
-      <c r="F24">
-        <v>25.31</v>
-      </c>
-      <c r="G24">
-        <v>41.75</v>
-      </c>
-      <c r="H24">
-        <v>11.83</v>
-      </c>
-      <c r="I24">
-        <v>74.786000000000001</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>74.592692307692303</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-      <c r="D25">
-        <v>8.9329999999999998</v>
-      </c>
-      <c r="E25">
-        <v>26.052600000000002</v>
-      </c>
-      <c r="F25">
-        <v>25.48</v>
-      </c>
-      <c r="G25">
-        <v>53.44</v>
-      </c>
-      <c r="H25">
-        <v>11.74</v>
-      </c>
-      <c r="I25">
-        <v>100.753</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>100.46884615384614</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>8.9369999999999994</v>
-      </c>
-      <c r="E26">
-        <v>26.037199999999999</v>
-      </c>
-      <c r="F26">
-        <v>25.49</v>
-      </c>
-      <c r="G26">
-        <v>53.48</v>
-      </c>
-      <c r="H26">
-        <v>11.74</v>
-      </c>
-      <c r="I26">
-        <v>100.6932</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>100.40961538461536</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{F66653EC-FEAC-4B99-B4F1-A71418C72B42}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0.20419999999999999</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>26.1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>E1:E26</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13627,15 +14050,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BB5143B-BA46-46F8-82D1-94F88A17AB4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17536349-18F2-47F9-B769-CFE5A50C8B29}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce4c9300-43b4-4cf5-a574-03edfaa98caf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13659,17 +14093,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17536349-18F2-47F9-B769-CFE5A50C8B29}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BB5143B-BA46-46F8-82D1-94F88A17AB4E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce4c9300-43b4-4cf5-a574-03edfaa98caf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>